<commit_message>
Added a predGDP title to the column of predictions.
</commit_message>
<xml_diff>
--- a/data/Excel Workbooks/JapanDataWorkbook.xlsx
+++ b/data/Excel Workbooks/JapanDataWorkbook.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="139">
   <si>
     <t>GDP [Millions of 1990$]</t>
   </si>
@@ -2228,7 +2228,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3607">
+  <cellStyleXfs count="3609">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -5845,6 +5845,8 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -6185,28 +6187,28 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6222,7 +6224,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3607">
+  <cellStyles count="3609">
     <cellStyle name="•\Ž¦Ï‚Ý‚ÌƒnƒCƒp[ƒŠƒ“ƒN" xfId="42"/>
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent1 10" xfId="54"/>
@@ -8286,6 +8288,7 @@
     <cellStyle name="Followed Hyperlink" xfId="3603" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3604" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3606" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3608" builtinId="9" hidden="1"/>
     <cellStyle name="ƒnƒCƒp[ƒŠƒ“ƒN" xfId="44"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Good 10" xfId="331"/>
@@ -8897,6 +8900,7 @@
     <cellStyle name="Hyperlink" xfId="3115" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3117" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3605" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3607" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink 10" xfId="898" hidden="1"/>
     <cellStyle name="Hyperlink 10" xfId="1133" hidden="1"/>
     <cellStyle name="Hyperlink 10" xfId="1337" hidden="1"/>
@@ -10585,7 +10589,7 @@
                   <c:v>0.906745398136488</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.0</c:v>
+                  <c:v>0.878955416963687</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11247,11 +11251,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2145658776"/>
-        <c:axId val="-2145653160"/>
+        <c:axId val="-2142568216"/>
+        <c:axId val="-2144736760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2145658776"/>
+        <c:axId val="-2142568216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2015.0"/>
@@ -11275,18 +11279,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145653160"/>
+        <c:crossAx val="-2144736760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2145653160"/>
+        <c:axId val="-2144736760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -11323,7 +11328,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145658776"/>
+        <c:crossAx val="-2142568216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1.0"/>
@@ -12269,11 +12274,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2146529048"/>
-        <c:axId val="-2146520648"/>
+        <c:axId val="-2144544232"/>
+        <c:axId val="-2144536216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2146529048"/>
+        <c:axId val="-2144544232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2011.0"/>
@@ -12303,13 +12308,13 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146520648"/>
+        <c:crossAx val="-2144536216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2146520648"/>
+        <c:axId val="-2144536216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12342,7 +12347,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146529048"/>
+        <c:crossAx val="-2144544232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13395,11 +13400,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2146471080"/>
-        <c:axId val="-2146462840"/>
+        <c:axId val="-2144486888"/>
+        <c:axId val="-2144478808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2146471080"/>
+        <c:axId val="-2144486888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2011.0"/>
@@ -13429,13 +13434,13 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146462840"/>
+        <c:crossAx val="-2144478808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2146462840"/>
+        <c:axId val="-2144478808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13468,7 +13473,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146471080"/>
+        <c:crossAx val="-2144486888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13488,7 +13493,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="102" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -13521,7 +13526,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8661400" cy="6286500"/>
+    <xdr:ext cx="8578725" cy="5827059"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -14270,7 +14275,7 @@
   <dimension ref="A1:AI46"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C9"/>
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -14564,7 +14569,7 @@
         <v>1.0293342659267073</v>
       </c>
       <c r="J11" s="25">
-        <f t="shared" ref="J11:J40" si="2">C11/$C$10</f>
+        <f t="shared" ref="J11:J41" si="2">C11/$C$10</f>
         <v>1.0029916611789609</v>
       </c>
       <c r="K11" s="125">
@@ -16061,8 +16066,9 @@
         <f t="shared" si="1"/>
         <v>1.7597635646470668</v>
       </c>
-      <c r="J41" s="25" t="s">
-        <v>129</v>
+      <c r="J41" s="125">
+        <f t="shared" si="2"/>
+        <v>0.8789554169636874</v>
       </c>
       <c r="K41" s="125">
         <f t="shared" si="3"/>
@@ -16154,18 +16160,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="L8:L9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="D8:D9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="L8:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -17386,9 +17392,9 @@
         <f>'Japan Workbook'!I41</f>
         <v>1.7597635646470668</v>
       </c>
-      <c r="D33" s="141" t="str">
+      <c r="D33" s="141">
         <f>'Japan Workbook'!J41</f>
-        <v>NA</v>
+        <v>0.8789554169636874</v>
       </c>
       <c r="E33" s="141">
         <f>'Japan Workbook'!K41</f>
@@ -18336,140 +18342,140 @@
       <c r="AG27" s="58"/>
     </row>
     <row r="28" spans="1:33" ht="15" customHeight="1">
-      <c r="A28" s="144" t="s">
+      <c r="A28" s="148" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="146" t="s">
+      <c r="B28" s="144" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="148" t="s">
+      <c r="C28" s="150" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="146" t="s">
+      <c r="D28" s="144" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="146" t="s">
+      <c r="E28" s="144" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="146" t="s">
+      <c r="F28" s="144" t="s">
         <v>48</v>
       </c>
-      <c r="G28" s="146" t="s">
+      <c r="G28" s="144" t="s">
         <v>49</v>
       </c>
-      <c r="H28" s="146" t="s">
+      <c r="H28" s="144" t="s">
         <v>60</v>
       </c>
-      <c r="I28" s="146" t="s">
+      <c r="I28" s="144" t="s">
         <v>61</v>
       </c>
-      <c r="J28" s="146" t="s">
+      <c r="J28" s="144" t="s">
         <v>68</v>
       </c>
-      <c r="K28" s="146" t="s">
+      <c r="K28" s="144" t="s">
         <v>69</v>
       </c>
-      <c r="L28" s="144" t="s">
+      <c r="L28" s="148" t="s">
         <v>55</v>
       </c>
-      <c r="M28" s="148" t="s">
+      <c r="M28" s="150" t="s">
         <v>50</v>
       </c>
-      <c r="N28" s="146" t="s">
+      <c r="N28" s="144" t="s">
         <v>51</v>
       </c>
-      <c r="O28" s="146" t="s">
+      <c r="O28" s="144" t="s">
         <v>90</v>
       </c>
-      <c r="P28" s="144" t="s">
+      <c r="P28" s="148" t="s">
         <v>28</v>
       </c>
-      <c r="Q28" s="148" t="s">
+      <c r="Q28" s="150" t="s">
         <v>29</v>
       </c>
-      <c r="R28" s="146" t="s">
+      <c r="R28" s="144" t="s">
         <v>30</v>
       </c>
-      <c r="S28" s="146" t="s">
+      <c r="S28" s="144" t="s">
         <v>31</v>
       </c>
-      <c r="T28" s="146" t="s">
+      <c r="T28" s="144" t="s">
         <v>32</v>
       </c>
-      <c r="U28" s="146" t="s">
+      <c r="U28" s="144" t="s">
         <v>52</v>
       </c>
-      <c r="V28" s="146" t="s">
+      <c r="V28" s="144" t="s">
         <v>67</v>
       </c>
-      <c r="W28" s="146" t="s">
+      <c r="W28" s="144" t="s">
         <v>79</v>
       </c>
-      <c r="X28" s="150" t="s">
+      <c r="X28" s="146" t="s">
         <v>33</v>
       </c>
-      <c r="Y28" s="144" t="s">
+      <c r="Y28" s="148" t="s">
         <v>81</v>
       </c>
-      <c r="Z28" s="148" t="s">
+      <c r="Z28" s="150" t="s">
         <v>82</v>
       </c>
-      <c r="AA28" s="146" t="s">
+      <c r="AA28" s="144" t="s">
         <v>83</v>
       </c>
-      <c r="AB28" s="146" t="s">
+      <c r="AB28" s="144" t="s">
         <v>84</v>
       </c>
-      <c r="AC28" s="146" t="s">
+      <c r="AC28" s="144" t="s">
         <v>85</v>
       </c>
-      <c r="AD28" s="146" t="s">
+      <c r="AD28" s="144" t="s">
         <v>86</v>
       </c>
-      <c r="AE28" s="146" t="s">
+      <c r="AE28" s="144" t="s">
         <v>87</v>
       </c>
-      <c r="AF28" s="146" t="s">
+      <c r="AF28" s="144" t="s">
         <v>88</v>
       </c>
-      <c r="AG28" s="150" t="s">
+      <c r="AG28" s="146" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:33">
-      <c r="A29" s="145"/>
-      <c r="B29" s="147"/>
-      <c r="C29" s="149"/>
-      <c r="D29" s="147"/>
-      <c r="E29" s="147"/>
-      <c r="F29" s="147"/>
-      <c r="G29" s="147"/>
-      <c r="H29" s="147"/>
-      <c r="I29" s="147"/>
-      <c r="J29" s="147"/>
-      <c r="K29" s="147"/>
-      <c r="L29" s="145"/>
-      <c r="M29" s="149"/>
-      <c r="N29" s="147"/>
-      <c r="O29" s="147"/>
-      <c r="P29" s="145"/>
-      <c r="Q29" s="149"/>
-      <c r="R29" s="147"/>
-      <c r="S29" s="147"/>
-      <c r="T29" s="147"/>
-      <c r="U29" s="147"/>
-      <c r="V29" s="147"/>
-      <c r="W29" s="147"/>
-      <c r="X29" s="151"/>
-      <c r="Y29" s="145"/>
-      <c r="Z29" s="149"/>
-      <c r="AA29" s="147"/>
-      <c r="AB29" s="147"/>
-      <c r="AC29" s="147"/>
-      <c r="AD29" s="147"/>
-      <c r="AE29" s="147"/>
-      <c r="AF29" s="147"/>
-      <c r="AG29" s="151"/>
+      <c r="A29" s="149"/>
+      <c r="B29" s="145"/>
+      <c r="C29" s="151"/>
+      <c r="D29" s="145"/>
+      <c r="E29" s="145"/>
+      <c r="F29" s="145"/>
+      <c r="G29" s="145"/>
+      <c r="H29" s="145"/>
+      <c r="I29" s="145"/>
+      <c r="J29" s="145"/>
+      <c r="K29" s="145"/>
+      <c r="L29" s="149"/>
+      <c r="M29" s="151"/>
+      <c r="N29" s="145"/>
+      <c r="O29" s="145"/>
+      <c r="P29" s="149"/>
+      <c r="Q29" s="151"/>
+      <c r="R29" s="145"/>
+      <c r="S29" s="145"/>
+      <c r="T29" s="145"/>
+      <c r="U29" s="145"/>
+      <c r="V29" s="145"/>
+      <c r="W29" s="145"/>
+      <c r="X29" s="147"/>
+      <c r="Y29" s="149"/>
+      <c r="Z29" s="151"/>
+      <c r="AA29" s="145"/>
+      <c r="AB29" s="145"/>
+      <c r="AC29" s="145"/>
+      <c r="AD29" s="145"/>
+      <c r="AE29" s="145"/>
+      <c r="AF29" s="145"/>
+      <c r="AG29" s="147"/>
     </row>
     <row r="30" spans="1:33">
       <c r="A30" s="40">
@@ -22235,24 +22241,11 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="AD28:AD29"/>
-    <mergeCell ref="AE28:AE29"/>
-    <mergeCell ref="AF28:AF29"/>
-    <mergeCell ref="AG28:AG29"/>
-    <mergeCell ref="Y28:Y29"/>
-    <mergeCell ref="Z28:Z29"/>
-    <mergeCell ref="AA28:AA29"/>
-    <mergeCell ref="AB28:AB29"/>
-    <mergeCell ref="AC28:AC29"/>
-    <mergeCell ref="X28:X29"/>
-    <mergeCell ref="P28:P29"/>
-    <mergeCell ref="Q28:Q29"/>
-    <mergeCell ref="R28:R29"/>
-    <mergeCell ref="S28:S29"/>
-    <mergeCell ref="T28:T29"/>
-    <mergeCell ref="U28:U29"/>
-    <mergeCell ref="V28:V29"/>
-    <mergeCell ref="W28:W29"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="M28:M29"/>
     <mergeCell ref="N28:N29"/>
     <mergeCell ref="O28:O29"/>
     <mergeCell ref="E28:E29"/>
@@ -22263,11 +22256,24 @@
     <mergeCell ref="J28:J29"/>
     <mergeCell ref="K28:K29"/>
     <mergeCell ref="L28:L29"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="X28:X29"/>
+    <mergeCell ref="P28:P29"/>
+    <mergeCell ref="Q28:Q29"/>
+    <mergeCell ref="R28:R29"/>
+    <mergeCell ref="S28:S29"/>
+    <mergeCell ref="T28:T29"/>
+    <mergeCell ref="U28:U29"/>
+    <mergeCell ref="V28:V29"/>
+    <mergeCell ref="W28:W29"/>
+    <mergeCell ref="AD28:AD29"/>
+    <mergeCell ref="AE28:AE29"/>
+    <mergeCell ref="AF28:AF29"/>
+    <mergeCell ref="AG28:AG29"/>
+    <mergeCell ref="Y28:Y29"/>
+    <mergeCell ref="Z28:Z29"/>
+    <mergeCell ref="AA28:AA29"/>
+    <mergeCell ref="AB28:AB29"/>
+    <mergeCell ref="AC28:AC29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>